<commit_message>
Move two cases from training set to test set
</commit_message>
<xml_diff>
--- a/K_testing_stand.xlsx
+++ b/K_testing_stand.xlsx
@@ -66,7 +66,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -87,11 +87,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -159,23 +154,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -196,10 +191,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L22" activeCellId="0" sqref="L22"/>
+      <selection pane="topLeft" activeCell="H22" activeCellId="0" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -209,7 +204,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="4.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.42"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.84"/>
@@ -542,78 +537,150 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="A10" s="0" t="n">
+        <v>0.074284</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>3.864</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>1.4486</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <f aca="false">(C10 - 0.5236)/1.0472</f>
+        <v>0.883307868601986</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <f aca="false">(E10 - 3) / 6</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="H10" s="1" t="n">
+        <f aca="false">(G10 - 2) / 2</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <f aca="false">(I10 - 0.0001) / 0.0099</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>0.03966</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>3.303</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>1.2043</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <f aca="false">(C11 - 0.5236)/1.0472</f>
+        <v>0.65001909854851</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <f aca="false">(E11 - 3) / 6</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <f aca="false">(G11 - 2) / 2</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="J11" s="1" t="n">
+        <f aca="false">(I11 - 0.0001) / 0.0099</f>
+        <v>1</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>387.2</v>
+      </c>
+    </row>
+    <row r="13" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J13" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" s="5" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+    <row r="15" s="5" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="6" t="n">
+      <c r="D15" s="6" t="n">
         <f aca="false">MIN(D1:D9)</f>
         <v>0</v>
       </c>
-      <c r="F13" s="6" t="n">
+      <c r="F15" s="6" t="n">
         <f aca="false">MIN(F1:F9)</f>
         <v>0</v>
       </c>
-      <c r="H13" s="6" t="n">
+      <c r="H15" s="6" t="n">
         <f aca="false">MIN(H1:H9)</f>
         <v>0</v>
       </c>
-      <c r="J13" s="6" t="n">
+      <c r="J15" s="6" t="n">
         <f aca="false">MIN(J1:J9)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" s="5" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
+    <row r="16" s="5" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="6" t="n">
+      <c r="D16" s="6" t="n">
         <f aca="false">MAX(D1:D9)</f>
         <v>1</v>
       </c>
-      <c r="F14" s="6" t="n">
+      <c r="F16" s="6" t="n">
         <f aca="false">MAX(F1:F9)</f>
         <v>1</v>
       </c>
-      <c r="H14" s="6" t="n">
+      <c r="H16" s="6" t="n">
         <f aca="false">MAX(H1:H9)</f>
         <v>1</v>
       </c>
-      <c r="J14" s="6" t="n">
+      <c r="J16" s="6" t="n">
         <f aca="false">MAX(J1:J9)</f>
         <v>1</v>
       </c>

</xml_diff>